<commit_message>
added missing columns in transport opt plus sample data
</commit_message>
<xml_diff>
--- a/pyloghub/sample_data/transportPlusAddresses.xlsx
+++ b/pyloghub/sample_data/transportPlusAddresses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\log-hub\log_hub\sample_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\log-hub-python\pyloghub\sample_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC3E562-AE48-4EC3-9D61-1775EFB17B3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1A6CFA-D9B6-41A3-9DC3-E4244433F0EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{9B4650FE-22C7-4596-BEDB-D8F3606EFAAD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="3" xr2:uid="{9B4650FE-22C7-4596-BEDB-D8F3606EFAAD}"/>
   </bookViews>
   <sheets>
     <sheet name="vehicles" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="132">
   <si>
     <t>Standard</t>
   </si>
@@ -408,16 +408,49 @@
   </si>
   <si>
     <t>breakDuration</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>perKilometer</t>
+  </si>
+  <si>
+    <t>costPerStop</t>
+  </si>
+  <si>
+    <t>minimumTravelTime</t>
+  </si>
+  <si>
+    <t>max_distance</t>
+  </si>
+  <si>
+    <t>maximumDistanceBetweenStops</t>
+  </si>
+  <si>
+    <t>earliestRelativeBreakStart</t>
+  </si>
+  <si>
+    <t>latestRelativeBreakStart</t>
+  </si>
+  <si>
+    <t>external_costs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -470,7 +503,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -478,28 +511,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="10">
     <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm"/>
+      <numFmt numFmtId="26" formatCode="h:mm:ss"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm"/>
+      <numFmt numFmtId="26" formatCode="h:mm:ss"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm"/>
+      <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm"/>
+      <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm"/>
+      <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm"/>
+      <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -521,16 +562,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D5603C8E-BC94-49CD-BAE1-FD7E0AA9BA2C}" name="Table16" displayName="Table16" ref="A1:AA4" totalsRowShown="0">
-  <autoFilter ref="A1:AA4" xr:uid="{D5603C8E-BC94-49CD-BAE1-FD7E0AA9BA2C}"/>
-  <tableColumns count="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D5603C8E-BC94-49CD-BAE1-FD7E0AA9BA2C}" name="Table16" displayName="Table16" ref="A1:AF4" totalsRowShown="0">
+  <autoFilter ref="A1:AF4" xr:uid="{D5603C8E-BC94-49CD-BAE1-FD7E0AA9BA2C}"/>
+  <tableColumns count="32">
     <tableColumn id="1" xr3:uid="{B7CD231C-A66F-4CAC-A48B-3E8F68A541D4}" name="id"/>
     <tableColumn id="27" xr3:uid="{7E98722D-34DE-4BD6-999A-17DAF25CCC45}" name="vehicleTypeId"/>
     <tableColumn id="2" xr3:uid="{70AC5862-B1DD-4D1C-A716-68F93AB2A0D1}" name="availableVehicles"/>
     <tableColumn id="3" xr3:uid="{2718CA4A-C472-4B9B-AC46-4C4A4CB71C83}" name="startId"/>
     <tableColumn id="4" xr3:uid="{32B3E45D-44A5-49FE-A719-63778E6227A9}" name="startCountry"/>
-    <tableColumn id="5" xr3:uid="{3DD7541D-535F-4877-BC40-594854EC6FF8}" name="startState" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{CE37A2E9-FCA6-45E3-ABA1-9AB7EAC2CF7A}" name="startPostalCode" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{3DD7541D-535F-4877-BC40-594854EC6FF8}" name="startState" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{CE37A2E9-FCA6-45E3-ABA1-9AB7EAC2CF7A}" name="startPostalCode" dataDxfId="8"/>
     <tableColumn id="7" xr3:uid="{EB7A3084-E1F8-4DF5-89F6-1C35A39585ED}" name="startCity"/>
     <tableColumn id="8" xr3:uid="{35C6FEA8-CEE1-4639-998C-794198DD5680}" name="startStreet"/>
     <tableColumn id="9" xr3:uid="{2C860987-4CBE-486E-9090-6D2478BA1376}" name="endId"/>
@@ -543,13 +584,18 @@
     <tableColumn id="16" xr3:uid="{0B9E0129-0ABC-49EB-8164-58132C1C5D80}" name="maxVolume"/>
     <tableColumn id="17" xr3:uid="{5D134840-58C8-45EA-AAB1-EAD24126C0DA}" name="maxPallets"/>
     <tableColumn id="18" xr3:uid="{5A1C9524-9990-4B77-93AA-3F410C4A7CBF}" name="maxStops"/>
-    <tableColumn id="19" xr3:uid="{3077E329-CA2C-4D6D-A03B-32D67AF41E72}" name="timeWindowStart" dataDxfId="5"/>
-    <tableColumn id="20" xr3:uid="{6839C7A3-8936-46E2-BE5F-1BEB00DB378F}" name="timeWindowEnd" dataDxfId="4"/>
+    <tableColumn id="19" xr3:uid="{3077E329-CA2C-4D6D-A03B-32D67AF41E72}" name="timeWindowStart" dataDxfId="7"/>
+    <tableColumn id="20" xr3:uid="{6839C7A3-8936-46E2-BE5F-1BEB00DB378F}" name="timeWindowEnd" dataDxfId="6"/>
     <tableColumn id="21" xr3:uid="{D105E071-1D22-454B-BDFD-5CEF4A5C20F4}" name="profile"/>
     <tableColumn id="22" xr3:uid="{A062B170-364F-4FDB-96CC-81740AA8DE4D}" name="speedFactor"/>
     <tableColumn id="23" xr3:uid="{693E5D2F-BB5D-42DB-A711-BC1543C15801}" name="fixed"/>
     <tableColumn id="24" xr3:uid="{7EC4276D-B23F-43B9-943A-345156B3AF2D}" name="perHour"/>
+    <tableColumn id="28" xr3:uid="{7334A817-0B1D-4546-853A-20FB795F7447}" name="perKilometer"/>
+    <tableColumn id="29" xr3:uid="{1413642E-8AD8-4C35-AC28-3932DC2A38D6}" name="costPerStop"/>
+    <tableColumn id="30" xr3:uid="{C2AB3B39-784C-4C85-A2AD-AF9B73D65BEC}" name="minimumTravelTime"/>
     <tableColumn id="25" xr3:uid="{9692B93D-2C5B-49DC-95ED-BAA6D22F3D04}" name="maxTravelTime"/>
+    <tableColumn id="32" xr3:uid="{16D66BA7-A9C8-4225-A0A5-F83B5D522992}" name="max_distance"/>
+    <tableColumn id="31" xr3:uid="{53C7D495-6B15-45F1-9016-5044759B8A17}" name="maximumDistanceBetweenStops"/>
     <tableColumn id="26" xr3:uid="{7F8AEA1A-06CA-4AF9-BE89-A4BC092AB357}" name="breakId"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -557,13 +603,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{6A02CD84-BD82-4A2E-9335-465DA1D0715C}" name="Table49" displayName="Table49" ref="A1:E2" totalsRowShown="0">
-  <autoFilter ref="A1:E2" xr:uid="{6A02CD84-BD82-4A2E-9335-465DA1D0715C}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{6A02CD84-BD82-4A2E-9335-465DA1D0715C}" name="Table49" displayName="Table49" ref="A1:G5" totalsRowShown="0">
+  <autoFilter ref="A1:G5" xr:uid="{6A02CD84-BD82-4A2E-9335-465DA1D0715C}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{322D61B1-D2BC-47A0-9201-A094D934B622}" name="id"/>
     <tableColumn id="5" xr3:uid="{4F2E4D02-9522-4A11-8FB4-DFE1C59D36E6}" name="breakId"/>
     <tableColumn id="2" xr3:uid="{98F162BE-DCDD-4718-9B17-ED0EA1E3F66F}" name="earliestBreakStart" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{C37BDEFD-495E-4A28-88AB-79A7A176022C}" name="latestBreakStart" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{7114990C-49D5-4873-9617-C284A154698C}" name="earliestRelativeBreakStart" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{F5EBAAE0-4D77-4E5C-8CD0-29741EF756AD}" name="latestRelativeBreakStart" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{72C9BC9A-AC62-429E-82A1-5B66BBC828E1}" name="breakDuration"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -571,9 +619,9 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{A049CF09-BED7-451E-99C5-2B3A95AF72CD}" name="Table37" displayName="Table37" ref="A1:V20" totalsRowShown="0">
-  <autoFilter ref="A1:V20" xr:uid="{A049CF09-BED7-451E-99C5-2B3A95AF72CD}"/>
-  <tableColumns count="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{A049CF09-BED7-451E-99C5-2B3A95AF72CD}" name="Table37" displayName="Table37" ref="A1:W20" totalsRowShown="0">
+  <autoFilter ref="A1:W20" xr:uid="{A049CF09-BED7-451E-99C5-2B3A95AF72CD}"/>
+  <tableColumns count="23">
     <tableColumn id="1" xr3:uid="{4FC4E853-0A94-439C-990D-4D097FDD5BBA}" name="id"/>
     <tableColumn id="22" xr3:uid="{774AB32C-5A52-41C1-8CDB-7EF54E9F47C2}" name="shipmentId"/>
     <tableColumn id="2" xr3:uid="{C547D106-2921-4E65-A748-3209026C9093}" name="fromName"/>
@@ -596,6 +644,7 @@
     <tableColumn id="19" xr3:uid="{AFA7A65E-A7E9-49EE-99F1-8CAEC8D9FBB8}" name="volume"/>
     <tableColumn id="20" xr3:uid="{3A20C5DE-AC33-43F4-BDE6-A48864D0BBF8}" name="pallets"/>
     <tableColumn id="21" xr3:uid="{90D3331C-6F90-45A7-991E-A593E5602587}" name="vehicleTypeId"/>
+    <tableColumn id="23" xr3:uid="{9408C912-0851-4846-9DBC-A834E0B539EE}" name="external_costs"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -607,17 +656,17 @@
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{CB6919D9-4088-432E-9250-8A6857130701}" name="id"/>
     <tableColumn id="4" xr3:uid="{34006944-BF30-42EA-B33E-17DB2B48B529}" name="timeWindowProfileId"/>
-    <tableColumn id="2" xr3:uid="{BFE5CD0D-BC86-41F3-BD2A-4F53BC527664}" name="timeWindowProfileStart" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{5DB8FCEC-1DEF-4CF8-9F7C-914AC90914C1}" name="timeWindowProfileEnd" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{BFE5CD0D-BC86-41F3-BD2A-4F53BC527664}" name="timeWindowProfileStart" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{5DB8FCEC-1DEF-4CF8-9F7C-914AC90914C1}" name="timeWindowProfileEnd" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -655,7 +704,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -761,7 +810,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -903,7 +952,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -911,7 +960,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="438" row="1">
+  <wetp:taskpane dockstate="right" visibility="0" width="438" row="5">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -922,16 +971,32 @@
   <we:reference id="e504fb41-a92a-4526-b101-542f357b7983" version="1.0.0.0" store="\\DESKTOP-OIBRO4V\Users\PC\Documents\Manifest" storeType="Filesystem"/>
   <we:alternateReferences/>
   <we:properties>
+    <we:property name="14_1breaks" value="&quot;5dcd4795-83339e84-46d77010&quot;"/>
+    <we:property name="14_1jobs" value="&quot;05e485e5-ce835f24-1aafe29f&quot;"/>
+    <we:property name="14_1timeWindowProfiles" value="&quot;1d37368e-fff9100a-15e7fc1f&quot;"/>
     <we:property name="14_1vehicles" value="&quot;4ee13575-5f42ef13-7ad03ea6&quot;"/>
-    <we:property name="14_1timeWindowProfiles" value="&quot;1d37368e-fff9100a-15e7fc1f&quot;"/>
-    <we:property name="14_1jobs" value="&quot;05e485e5-ce835f24-1aafe29f&quot;"/>
-    <we:property name="14_1breaks" value="&quot;5dcd4795-83339e84-46d77010&quot;"/>
+    <we:property name="2_3vehicles" value="&quot;22849af7-7fb23345-542ab120&quot;"/>
+    <we:property name="2_3jobs" value="&quot;785d9f92-506bb200-dff76137&quot;"/>
+    <we:property name="2_3timeWindowProfiles" value="&quot;dd8347ad-5b2e048f-0bb33840&quot;"/>
+    <we:property name="2_3breaks" value="&quot;b3d706a1-5cd5c5a2-ccd63413&quot;"/>
+    <we:property name="2_3routeOverview" value="&quot;1f1cd397-e131f1c5-b7aa694f&quot;"/>
+    <we:property name="2_3routeDetails" value="&quot;bcc8d540-34d4e389-56fec290&quot;"/>
+    <we:property name="2_3droppedCustomers" value="&quot;1d1b9b90-a1c04872-a5816a96&quot;"/>
+    <we:property name="2_3parameters" value="&quot;e862fe50-e6605013-f08580bd&quot;"/>
   </we:properties>
   <we:bindings>
     <we:binding id="4ee13575-5f42ef13-7ad03ea6" type="table" appref="{525B8A55-3DA7-4705-BB34-BA70DF273048}"/>
     <we:binding id="1d37368e-fff9100a-15e7fc1f" type="table" appref="{33F80202-D383-4897-9932-A816E2E794CC}"/>
     <we:binding id="05e485e5-ce835f24-1aafe29f" type="table" appref="{67E6975F-4B4F-4CF5-B1DD-6CD7EC695932}"/>
     <we:binding id="5dcd4795-83339e84-46d77010" type="table" appref="{2F7E2EC6-E112-4597-982E-AED9311E9C61}"/>
+    <we:binding id="22849af7-7fb23345-542ab120" type="table" appref="{5F0F5684-10C9-4439-AAD7-C61EFE90CCEC}"/>
+    <we:binding id="785d9f92-506bb200-dff76137" type="table" appref="{9FAC752E-5F17-41FD-8AF7-6DA3677CFB5D}"/>
+    <we:binding id="dd8347ad-5b2e048f-0bb33840" type="table" appref="{DEDE07BF-AB2F-4300-AE18-E8C520082494}"/>
+    <we:binding id="b3d706a1-5cd5c5a2-ccd63413" type="table" appref="{A883CC5E-5396-4B62-A438-A81B9735F684}"/>
+    <we:binding id="1f1cd397-e131f1c5-b7aa694f" type="table" appref="{599CA4EF-96C0-423F-BB08-454005D9E35D}"/>
+    <we:binding id="bcc8d540-34d4e389-56fec290" type="table" appref="{0699398F-3B06-4BD5-B9CF-2EA66147FE66}"/>
+    <we:binding id="1d1b9b90-a1c04872-a5816a96" type="table" appref="{7C1BF460-071E-45FB-8913-DC7265844087}"/>
+    <we:binding id="e862fe50-e6605013-f08580bd" type="table" appref="{78B0E116-9ABB-4542-9A15-20F1161F31FE}"/>
   </we:bindings>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </we:webextension>
@@ -939,44 +1004,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3DB5624-E631-452E-A435-626226692B26}">
-  <dimension ref="A1:AA4"/>
+  <dimension ref="A1:AF4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="B2" sqref="B2:AF4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.6328125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.21875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.08984375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.6328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.36328125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.54296875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.90625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:32" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>70</v>
       </c>
@@ -1053,13 +1118,28 @@
         <v>94</v>
       </c>
       <c r="Z1" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="AC1" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="AF1" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1075,7 +1155,10 @@
       <c r="E2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
         <v>3</v>
       </c>
       <c r="H2" t="s">
@@ -1090,6 +1173,12 @@
       <c r="K2" t="s">
         <v>2</v>
       </c>
+      <c r="L2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" t="s">
+        <v>3</v>
+      </c>
       <c r="N2" t="s">
         <v>4</v>
       </c>
@@ -1127,13 +1216,28 @@
         <v>30</v>
       </c>
       <c r="Z2">
-        <v>1200</v>
-      </c>
-      <c r="AA2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA2">
+        <v>2</v>
+      </c>
+      <c r="AB2">
+        <v>2</v>
+      </c>
+      <c r="AC2">
+        <v>1000</v>
+      </c>
+      <c r="AD2">
+        <v>1000</v>
+      </c>
+      <c r="AE2">
+        <v>400</v>
+      </c>
+      <c r="AF2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1149,7 +1253,10 @@
       <c r="E3" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
         <v>3</v>
       </c>
       <c r="H3" t="s">
@@ -1164,6 +1271,12 @@
       <c r="K3" t="s">
         <v>2</v>
       </c>
+      <c r="L3" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" t="s">
+        <v>3</v>
+      </c>
       <c r="N3" t="s">
         <v>4</v>
       </c>
@@ -1201,13 +1314,28 @@
         <v>30</v>
       </c>
       <c r="Z3">
-        <v>1200</v>
-      </c>
-      <c r="AA3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA3">
+        <v>2</v>
+      </c>
+      <c r="AB3">
+        <v>2</v>
+      </c>
+      <c r="AC3">
+        <v>1000</v>
+      </c>
+      <c r="AD3">
+        <v>1000</v>
+      </c>
+      <c r="AE3">
+        <v>400</v>
+      </c>
+      <c r="AF3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1223,7 +1351,10 @@
       <c r="E4" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
         <v>3</v>
       </c>
       <c r="H4" t="s">
@@ -1238,6 +1369,12 @@
       <c r="K4" t="s">
         <v>2</v>
       </c>
+      <c r="L4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M4" t="s">
+        <v>3</v>
+      </c>
       <c r="N4" t="s">
         <v>4</v>
       </c>
@@ -1275,13 +1412,29 @@
         <v>30</v>
       </c>
       <c r="Z4">
-        <v>1200</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>7</v>
+        <v>1</v>
+      </c>
+      <c r="AA4">
+        <v>2</v>
+      </c>
+      <c r="AB4">
+        <v>2</v>
+      </c>
+      <c r="AC4">
+        <v>1000</v>
+      </c>
+      <c r="AD4">
+        <v>1000</v>
+      </c>
+      <c r="AE4">
+        <v>400</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -1309,22 +1462,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC009EB7-11A0-482B-AF76-5E915329C990}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1796875" customWidth="1"/>
-    <col min="3" max="3" width="19.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.21875" customWidth="1"/>
+    <col min="3" max="3" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>70</v>
       </c>
@@ -1338,10 +1491,16 @@
         <v>121</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1349,58 +1508,164 @@
         <v>7</v>
       </c>
       <c r="C2" s="1">
+        <v>44546.833333333299</v>
+      </c>
+      <c r="D2" s="1">
+        <v>44546.875</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1">
         <v>44546.916666666701</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D3" s="1">
         <v>44546.958333333299</v>
       </c>
-      <c r="E2">
+      <c r="E3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3">
         <v>30</v>
       </c>
     </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="7">
+        <v>8.3333333300000006E-2</v>
+      </c>
+      <c r="F4" s="7">
+        <v>0.16666666669999999</v>
+      </c>
+      <c r="G4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="F5" s="7">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G5">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{F7C9EE02-42E1-4005-9D12-6889AFFD525C}">
+      <x15:webExtensions xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x15:webExtension appRef="{5F0F5684-10C9-4439-AAD7-C61EFE90CCEC}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{9FAC752E-5F17-41FD-8AF7-6DA3677CFB5D}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{DEDE07BF-AB2F-4300-AE18-E8C520082494}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{A883CC5E-5396-4B62-A438-A81B9735F684}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{599CA4EF-96C0-423F-BB08-454005D9E35D}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{0699398F-3B06-4BD5-B9CF-2EA66147FE66}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{7C1BF460-071E-45FB-8913-DC7265844087}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{78B0E116-9ABB-4542-9A15-20F1161F31FE}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+      </x15:webExtensions>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C0F778F-3E72-476C-9BC6-B1FE033292D5}">
-  <dimension ref="A1:V20"/>
+  <dimension ref="A1:W20"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2:V20"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:W20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.08984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="29.08984375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>70</v>
       </c>
@@ -1467,8 +1732,11 @@
       <c r="V1" s="4" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W1" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1481,9 +1749,18 @@
       <c r="D2" t="s">
         <v>2</v>
       </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
       <c r="G2" t="s">
         <v>14</v>
       </c>
+      <c r="H2" t="s">
+        <v>3</v>
+      </c>
       <c r="I2">
         <v>10</v>
       </c>
@@ -1496,9 +1773,18 @@
       <c r="L2" t="s">
         <v>2</v>
       </c>
+      <c r="M2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" t="s">
+        <v>3</v>
+      </c>
       <c r="O2" t="s">
         <v>15</v>
       </c>
+      <c r="P2" t="s">
+        <v>3</v>
+      </c>
       <c r="Q2">
         <v>15</v>
       </c>
@@ -1514,8 +1800,14 @@
       <c r="U2">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V2" t="s">
+        <v>3</v>
+      </c>
+      <c r="W2">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1528,9 +1820,18 @@
       <c r="D3" t="s">
         <v>2</v>
       </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
       <c r="G3" t="s">
         <v>17</v>
       </c>
+      <c r="H3" t="s">
+        <v>3</v>
+      </c>
       <c r="I3">
         <v>10</v>
       </c>
@@ -1543,9 +1844,18 @@
       <c r="L3" t="s">
         <v>2</v>
       </c>
+      <c r="M3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N3" t="s">
+        <v>3</v>
+      </c>
       <c r="O3" t="s">
         <v>18</v>
       </c>
+      <c r="P3" t="s">
+        <v>3</v>
+      </c>
       <c r="Q3">
         <v>15</v>
       </c>
@@ -1561,8 +1871,14 @@
       <c r="U3">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V3" t="s">
+        <v>3</v>
+      </c>
+      <c r="W3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1575,9 +1891,18 @@
       <c r="D4" t="s">
         <v>2</v>
       </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
       <c r="G4" t="s">
         <v>20</v>
       </c>
+      <c r="H4" t="s">
+        <v>3</v>
+      </c>
       <c r="I4">
         <v>10</v>
       </c>
@@ -1590,9 +1915,18 @@
       <c r="L4" t="s">
         <v>2</v>
       </c>
+      <c r="M4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N4" t="s">
+        <v>3</v>
+      </c>
       <c r="O4" t="s">
         <v>21</v>
       </c>
+      <c r="P4" t="s">
+        <v>3</v>
+      </c>
       <c r="Q4">
         <v>15</v>
       </c>
@@ -1608,8 +1942,14 @@
       <c r="U4">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V4" t="s">
+        <v>3</v>
+      </c>
+      <c r="W4">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1622,9 +1962,18 @@
       <c r="D5" t="s">
         <v>2</v>
       </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3</v>
+      </c>
       <c r="G5" t="s">
         <v>23</v>
       </c>
+      <c r="H5" t="s">
+        <v>3</v>
+      </c>
       <c r="I5">
         <v>10</v>
       </c>
@@ -1637,9 +1986,18 @@
       <c r="L5" t="s">
         <v>2</v>
       </c>
+      <c r="M5" t="s">
+        <v>3</v>
+      </c>
+      <c r="N5" t="s">
+        <v>3</v>
+      </c>
       <c r="O5" t="s">
         <v>24</v>
       </c>
+      <c r="P5" t="s">
+        <v>3</v>
+      </c>
       <c r="Q5">
         <v>15</v>
       </c>
@@ -1655,8 +2013,14 @@
       <c r="U5">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V5" t="s">
+        <v>3</v>
+      </c>
+      <c r="W5">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1669,9 +2033,18 @@
       <c r="D6" t="s">
         <v>2</v>
       </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>3</v>
+      </c>
       <c r="G6" t="s">
         <v>26</v>
       </c>
+      <c r="H6" t="s">
+        <v>3</v>
+      </c>
       <c r="I6">
         <v>10</v>
       </c>
@@ -1684,9 +2057,18 @@
       <c r="L6" t="s">
         <v>2</v>
       </c>
+      <c r="M6" t="s">
+        <v>3</v>
+      </c>
+      <c r="N6" t="s">
+        <v>3</v>
+      </c>
       <c r="O6" t="s">
         <v>27</v>
       </c>
+      <c r="P6" t="s">
+        <v>3</v>
+      </c>
       <c r="Q6">
         <v>15</v>
       </c>
@@ -1702,8 +2084,14 @@
       <c r="U6">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V6" t="s">
+        <v>3</v>
+      </c>
+      <c r="W6">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1716,9 +2104,18 @@
       <c r="D7" t="s">
         <v>2</v>
       </c>
+      <c r="E7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>3</v>
+      </c>
       <c r="G7" t="s">
         <v>29</v>
       </c>
+      <c r="H7" t="s">
+        <v>3</v>
+      </c>
       <c r="I7">
         <v>10</v>
       </c>
@@ -1731,9 +2128,18 @@
       <c r="L7" t="s">
         <v>2</v>
       </c>
+      <c r="M7" t="s">
+        <v>3</v>
+      </c>
+      <c r="N7" t="s">
+        <v>3</v>
+      </c>
       <c r="O7" t="s">
         <v>30</v>
       </c>
+      <c r="P7" t="s">
+        <v>3</v>
+      </c>
       <c r="Q7">
         <v>15</v>
       </c>
@@ -1749,8 +2155,14 @@
       <c r="U7">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V7" t="s">
+        <v>3</v>
+      </c>
+      <c r="W7">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1763,9 +2175,18 @@
       <c r="D8" t="s">
         <v>2</v>
       </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>3</v>
+      </c>
       <c r="G8" t="s">
         <v>32</v>
       </c>
+      <c r="H8" t="s">
+        <v>3</v>
+      </c>
       <c r="I8">
         <v>10</v>
       </c>
@@ -1778,9 +2199,18 @@
       <c r="L8" t="s">
         <v>2</v>
       </c>
+      <c r="M8" t="s">
+        <v>3</v>
+      </c>
+      <c r="N8" t="s">
+        <v>3</v>
+      </c>
       <c r="O8" t="s">
         <v>33</v>
       </c>
+      <c r="P8" t="s">
+        <v>3</v>
+      </c>
       <c r="Q8">
         <v>15</v>
       </c>
@@ -1796,8 +2226,14 @@
       <c r="U8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V8" t="s">
+        <v>3</v>
+      </c>
+      <c r="W8">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1810,9 +2246,18 @@
       <c r="D9" t="s">
         <v>2</v>
       </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>3</v>
+      </c>
       <c r="G9" t="s">
         <v>35</v>
       </c>
+      <c r="H9" t="s">
+        <v>3</v>
+      </c>
       <c r="I9">
         <v>10</v>
       </c>
@@ -1825,9 +2270,18 @@
       <c r="L9" t="s">
         <v>2</v>
       </c>
+      <c r="M9" t="s">
+        <v>3</v>
+      </c>
+      <c r="N9" t="s">
+        <v>3</v>
+      </c>
       <c r="O9" t="s">
         <v>36</v>
       </c>
+      <c r="P9" t="s">
+        <v>3</v>
+      </c>
       <c r="Q9">
         <v>15</v>
       </c>
@@ -1843,8 +2297,14 @@
       <c r="U9">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V9" t="s">
+        <v>3</v>
+      </c>
+      <c r="W9">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1857,9 +2317,18 @@
       <c r="D10" t="s">
         <v>2</v>
       </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>3</v>
+      </c>
       <c r="G10" t="s">
         <v>38</v>
       </c>
+      <c r="H10" t="s">
+        <v>3</v>
+      </c>
       <c r="I10">
         <v>10</v>
       </c>
@@ -1872,9 +2341,18 @@
       <c r="L10" t="s">
         <v>2</v>
       </c>
+      <c r="M10" t="s">
+        <v>3</v>
+      </c>
+      <c r="N10" t="s">
+        <v>3</v>
+      </c>
       <c r="O10" t="s">
         <v>39</v>
       </c>
+      <c r="P10" t="s">
+        <v>3</v>
+      </c>
       <c r="Q10">
         <v>15</v>
       </c>
@@ -1890,8 +2368,14 @@
       <c r="U10">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V10" t="s">
+        <v>3</v>
+      </c>
+      <c r="W10">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1904,9 +2388,18 @@
       <c r="D11" t="s">
         <v>2</v>
       </c>
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" t="s">
+        <v>3</v>
+      </c>
       <c r="G11" t="s">
         <v>41</v>
       </c>
+      <c r="H11" t="s">
+        <v>3</v>
+      </c>
       <c r="I11">
         <v>10</v>
       </c>
@@ -1919,9 +2412,18 @@
       <c r="L11" t="s">
         <v>2</v>
       </c>
+      <c r="M11" t="s">
+        <v>3</v>
+      </c>
+      <c r="N11" t="s">
+        <v>3</v>
+      </c>
       <c r="O11" t="s">
         <v>42</v>
       </c>
+      <c r="P11" t="s">
+        <v>3</v>
+      </c>
       <c r="Q11">
         <v>15</v>
       </c>
@@ -1937,8 +2439,14 @@
       <c r="U11">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V11" t="s">
+        <v>3</v>
+      </c>
+      <c r="W11">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1951,9 +2459,18 @@
       <c r="D12" t="s">
         <v>2</v>
       </c>
+      <c r="E12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" t="s">
+        <v>3</v>
+      </c>
       <c r="G12" t="s">
         <v>44</v>
       </c>
+      <c r="H12" t="s">
+        <v>3</v>
+      </c>
       <c r="I12">
         <v>10</v>
       </c>
@@ -1966,9 +2483,18 @@
       <c r="L12" t="s">
         <v>2</v>
       </c>
+      <c r="M12" t="s">
+        <v>3</v>
+      </c>
+      <c r="N12" t="s">
+        <v>3</v>
+      </c>
       <c r="O12" t="s">
         <v>45</v>
       </c>
+      <c r="P12" t="s">
+        <v>3</v>
+      </c>
       <c r="Q12">
         <v>15</v>
       </c>
@@ -1984,8 +2510,14 @@
       <c r="U12">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V12" t="s">
+        <v>3</v>
+      </c>
+      <c r="W12">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1998,9 +2530,18 @@
       <c r="D13" t="s">
         <v>2</v>
       </c>
+      <c r="E13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" t="s">
+        <v>3</v>
+      </c>
       <c r="G13" t="s">
         <v>47</v>
       </c>
+      <c r="H13" t="s">
+        <v>3</v>
+      </c>
       <c r="I13">
         <v>10</v>
       </c>
@@ -2013,9 +2554,18 @@
       <c r="L13" t="s">
         <v>2</v>
       </c>
+      <c r="M13" t="s">
+        <v>3</v>
+      </c>
+      <c r="N13" t="s">
+        <v>3</v>
+      </c>
       <c r="O13" t="s">
         <v>48</v>
       </c>
+      <c r="P13" t="s">
+        <v>3</v>
+      </c>
       <c r="Q13">
         <v>15</v>
       </c>
@@ -2031,8 +2581,14 @@
       <c r="U13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V13" t="s">
+        <v>3</v>
+      </c>
+      <c r="W13">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2045,9 +2601,18 @@
       <c r="D14" t="s">
         <v>2</v>
       </c>
+      <c r="E14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" t="s">
+        <v>3</v>
+      </c>
       <c r="G14" t="s">
         <v>50</v>
       </c>
+      <c r="H14" t="s">
+        <v>3</v>
+      </c>
       <c r="I14">
         <v>10</v>
       </c>
@@ -2060,9 +2625,18 @@
       <c r="L14" t="s">
         <v>2</v>
       </c>
+      <c r="M14" t="s">
+        <v>3</v>
+      </c>
+      <c r="N14" t="s">
+        <v>3</v>
+      </c>
       <c r="O14" t="s">
         <v>51</v>
       </c>
+      <c r="P14" t="s">
+        <v>3</v>
+      </c>
       <c r="Q14">
         <v>15</v>
       </c>
@@ -2078,8 +2652,14 @@
       <c r="U14">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V14" t="s">
+        <v>3</v>
+      </c>
+      <c r="W14">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2092,9 +2672,18 @@
       <c r="D15" t="s">
         <v>2</v>
       </c>
+      <c r="E15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" t="s">
+        <v>3</v>
+      </c>
       <c r="G15" t="s">
         <v>53</v>
       </c>
+      <c r="H15" t="s">
+        <v>3</v>
+      </c>
       <c r="I15">
         <v>10</v>
       </c>
@@ -2107,9 +2696,18 @@
       <c r="L15" t="s">
         <v>2</v>
       </c>
+      <c r="M15" t="s">
+        <v>3</v>
+      </c>
+      <c r="N15" t="s">
+        <v>3</v>
+      </c>
       <c r="O15" t="s">
         <v>54</v>
       </c>
+      <c r="P15" t="s">
+        <v>3</v>
+      </c>
       <c r="Q15">
         <v>15</v>
       </c>
@@ -2125,8 +2723,14 @@
       <c r="U15">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="V15" t="s">
+        <v>3</v>
+      </c>
+      <c r="W15">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2139,9 +2743,18 @@
       <c r="D16" t="s">
         <v>2</v>
       </c>
+      <c r="E16" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" t="s">
+        <v>3</v>
+      </c>
       <c r="G16" t="s">
         <v>56</v>
       </c>
+      <c r="H16" t="s">
+        <v>3</v>
+      </c>
       <c r="I16">
         <v>10</v>
       </c>
@@ -2154,9 +2767,18 @@
       <c r="L16" t="s">
         <v>2</v>
       </c>
+      <c r="M16" t="s">
+        <v>3</v>
+      </c>
+      <c r="N16" t="s">
+        <v>3</v>
+      </c>
       <c r="O16" t="s">
         <v>57</v>
       </c>
+      <c r="P16" t="s">
+        <v>3</v>
+      </c>
       <c r="Q16">
         <v>15</v>
       </c>
@@ -2172,8 +2794,14 @@
       <c r="U16">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V16" t="s">
+        <v>3</v>
+      </c>
+      <c r="W16">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2186,9 +2814,18 @@
       <c r="D17" t="s">
         <v>2</v>
       </c>
+      <c r="E17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" t="s">
+        <v>3</v>
+      </c>
       <c r="G17" t="s">
         <v>59</v>
       </c>
+      <c r="H17" t="s">
+        <v>3</v>
+      </c>
       <c r="I17">
         <v>10</v>
       </c>
@@ -2201,9 +2838,18 @@
       <c r="L17" t="s">
         <v>2</v>
       </c>
+      <c r="M17" t="s">
+        <v>3</v>
+      </c>
+      <c r="N17" t="s">
+        <v>3</v>
+      </c>
       <c r="O17" t="s">
         <v>60</v>
       </c>
+      <c r="P17" t="s">
+        <v>3</v>
+      </c>
       <c r="Q17">
         <v>15</v>
       </c>
@@ -2219,8 +2865,14 @@
       <c r="U17">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V17" t="s">
+        <v>3</v>
+      </c>
+      <c r="W17">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2233,9 +2885,18 @@
       <c r="D18" t="s">
         <v>2</v>
       </c>
+      <c r="E18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" t="s">
+        <v>3</v>
+      </c>
       <c r="G18" t="s">
         <v>62</v>
       </c>
+      <c r="H18" t="s">
+        <v>3</v>
+      </c>
       <c r="I18">
         <v>10</v>
       </c>
@@ -2248,9 +2909,18 @@
       <c r="L18" t="s">
         <v>2</v>
       </c>
+      <c r="M18" t="s">
+        <v>3</v>
+      </c>
+      <c r="N18" t="s">
+        <v>3</v>
+      </c>
       <c r="O18" t="s">
         <v>63</v>
       </c>
+      <c r="P18" t="s">
+        <v>3</v>
+      </c>
       <c r="Q18">
         <v>15</v>
       </c>
@@ -2266,8 +2936,14 @@
       <c r="U18">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V18" t="s">
+        <v>3</v>
+      </c>
+      <c r="W18">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2280,9 +2956,18 @@
       <c r="D19" t="s">
         <v>2</v>
       </c>
+      <c r="E19" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" t="s">
+        <v>3</v>
+      </c>
       <c r="G19" t="s">
         <v>65</v>
       </c>
+      <c r="H19" t="s">
+        <v>3</v>
+      </c>
       <c r="I19">
         <v>10</v>
       </c>
@@ -2295,9 +2980,18 @@
       <c r="L19" t="s">
         <v>2</v>
       </c>
+      <c r="M19" t="s">
+        <v>3</v>
+      </c>
+      <c r="N19" t="s">
+        <v>3</v>
+      </c>
       <c r="O19" t="s">
         <v>66</v>
       </c>
+      <c r="P19" t="s">
+        <v>3</v>
+      </c>
       <c r="Q19">
         <v>15</v>
       </c>
@@ -2313,8 +3007,14 @@
       <c r="U19">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="V19" t="s">
+        <v>3</v>
+      </c>
+      <c r="W19">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2327,9 +3027,18 @@
       <c r="D20" t="s">
         <v>2</v>
       </c>
+      <c r="E20" t="s">
+        <v>3</v>
+      </c>
+      <c r="F20" t="s">
+        <v>3</v>
+      </c>
       <c r="G20" t="s">
         <v>68</v>
       </c>
+      <c r="H20" t="s">
+        <v>3</v>
+      </c>
       <c r="I20">
         <v>10</v>
       </c>
@@ -2342,9 +3051,18 @@
       <c r="L20" t="s">
         <v>2</v>
       </c>
+      <c r="M20" t="s">
+        <v>3</v>
+      </c>
+      <c r="N20" t="s">
+        <v>3</v>
+      </c>
       <c r="O20" t="s">
         <v>69</v>
       </c>
+      <c r="P20" t="s">
+        <v>3</v>
+      </c>
       <c r="Q20">
         <v>15</v>
       </c>
@@ -2359,6 +3077,12 @@
       </c>
       <c r="U20">
         <v>3</v>
+      </c>
+      <c r="V20" t="s">
+        <v>3</v>
+      </c>
+      <c r="W20">
+        <v>2000</v>
       </c>
     </row>
   </sheetData>
@@ -2373,19 +3097,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE3A0BB0-C44F-443F-B2C4-340BDAC55EF6}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7265625" customWidth="1"/>
-    <col min="3" max="3" width="25.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.77734375" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>70</v>
       </c>
@@ -2399,7 +3123,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2413,7 +3137,7 @@
         <v>44547.020833333299</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2427,7 +3151,7 @@
         <v>44547.208333333299</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2441,7 +3165,7 @@
         <v>44547.333333333299</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2455,7 +3179,7 @@
         <v>44547.020833333299</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2469,7 +3193,7 @@
         <v>44547.208333333299</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>

</xml_diff>